<commit_message>
proto-board working, about to begin software dev for file input and plotting.
</commit_message>
<xml_diff>
--- a/Finances/Purchases.xlsx
+++ b/Finances/Purchases.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mufasa\Documents\Thesis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mufasa\Documents\Thesis\Finances\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="45">
   <si>
     <t>Supplier</t>
   </si>
@@ -138,6 +138,27 @@
   </si>
   <si>
     <t>125427-130930</t>
+  </si>
+  <si>
+    <t>Thesis v3.00BOB</t>
+  </si>
+  <si>
+    <t>Thesis v3.00</t>
+  </si>
+  <si>
+    <t>Pressure v2.00</t>
+  </si>
+  <si>
+    <t>Components for Thesis v3.00, Thesis v3.00BOB, and Pressure v2.00</t>
+  </si>
+  <si>
+    <t>ZuAWe6Su</t>
+  </si>
+  <si>
+    <t>FFjMkWOU</t>
+  </si>
+  <si>
+    <t>aF0dGEKE</t>
   </si>
 </sst>
 </file>
@@ -475,17 +496,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:E30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
     <col min="3" max="3" width="66.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="42.28515625" bestFit="1" customWidth="1"/>
@@ -773,13 +794,74 @@
         <v>76.34</v>
       </c>
     </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" t="s">
+        <v>44</v>
+      </c>
+    </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22">
+        <v>829749</v>
+      </c>
+      <c r="D22">
+        <v>147.21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23">
+        <v>43539112</v>
+      </c>
+      <c r="D23">
+        <v>177.91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
         <v>2</v>
       </c>
-      <c r="D22" s="1">
-        <f>SUM(D2:D20)</f>
-        <v>7612.68</v>
+      <c r="D30" s="1">
+        <f>SUM(D2:D27)</f>
+        <v>7937.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>